<commit_message>
Resolved interpreter conflicts in PyCharmProjects; relabeled and relocated pip3.9/pip3.12 artifacts
</commit_message>
<xml_diff>
--- a/filelist.xlsx
+++ b/filelist.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="List of Files" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="List of Files" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -140,13 +140,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -488,12 +488,12 @@
     <row r="3" ht="52" customHeight="1">
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-02-07 144957 switch_before_go.png</t>
+          <t>Screenshot 2023-03-15 084217.png</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2/7/2025 2:50:11 PM</t>
+          <t>3/15/2023 8:42:17 AM</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Filelist_workbook.py is fully functioning. Might add a struct class to it later.
</commit_message>
<xml_diff>
--- a/filelist.xlsx
+++ b/filelist.xlsx
@@ -9164,7 +9164,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>2025-07-16 11:04AM</t>
+          <t>2025 October 29 @03:29PM</t>
         </is>
       </c>
     </row>
@@ -9185,7 +9185,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="121" customHeight="1">
+    <row r="3" ht="39" customHeight="1">
       <c r="B3" t="inlineStr">
         <is>
           <t>2025-02-07 144957 switch_before_go.png</t>
@@ -9197,7 +9197,7 @@
         </is>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="41.25" customHeight="1">
       <c r="B4" t="inlineStr">
         <is>
           <t>cse100_lab4_BothPlayers_LOSE.png</t>
@@ -9209,7 +9209,7 @@
         </is>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="41.25" customHeight="1">
       <c r="B5" t="inlineStr">
         <is>
           <t>cse100_lab4_BothPlayers_WIN.png</t>
@@ -9221,7 +9221,7 @@
         </is>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="42.75" customHeight="1">
       <c r="B6" t="inlineStr">
         <is>
           <t>cse100_lab4_PlayerA_wins.png</t>
@@ -9233,7 +9233,7 @@
         </is>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="41.25" customHeight="1">
       <c r="B7" t="inlineStr">
         <is>
           <t>cse100_lab4_PlayerB_wins.png</t>
@@ -9245,7 +9245,7 @@
         </is>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="42.75" customHeight="1">
       <c r="B8" t="inlineStr">
         <is>
           <t>CSE100_Statemachine_question 2025-02-02 1050.png</t>
@@ -9257,7 +9257,7 @@
         </is>
       </c>
     </row>
-    <row r="9">
+    <row r="9" ht="58.5" customHeight="1">
       <c r="B9" t="inlineStr">
         <is>
           <t>CSE100_Statemachine_schematic.png</t>
@@ -9269,7 +9269,7 @@
         </is>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="81" customHeight="1">
       <c r="B10" t="inlineStr">
         <is>
           <t>CSE3_SCRATCHgame 2025-07-23 224218.png</t>
@@ -9281,7 +9281,7 @@
         </is>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="36" customHeight="1">
       <c r="B11" t="inlineStr">
         <is>
           <t>ECE118_20250403_1232.png</t>
@@ -9293,7 +9293,7 @@
         </is>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="28.5" customHeight="1">
       <c r="B12" t="inlineStr">
         <is>
           <t>ECE118_20250403_1246.png</t>
@@ -9305,7 +9305,7 @@
         </is>
       </c>
     </row>
-    <row r="13">
+    <row r="13" ht="33" customHeight="1">
       <c r="B13" t="inlineStr">
         <is>
           <t>ECE118_20250403_1315.png</t>
@@ -9317,7 +9317,7 @@
         </is>
       </c>
     </row>
-    <row r="14">
+    <row r="14" ht="48" customHeight="1">
       <c r="B14" t="inlineStr">
         <is>
           <t>IMG_0639.PNG</t>
@@ -9329,7 +9329,7 @@
         </is>
       </c>
     </row>
-    <row r="15">
+    <row r="15" ht="40.5" customHeight="1">
       <c r="B15" t="inlineStr">
         <is>
           <t>IMG_20250301_111833072.png</t>
@@ -9341,7 +9341,7 @@
         </is>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="96.75" customHeight="1">
       <c r="B16" t="inlineStr">
         <is>
           <t>Lab2_CAD-drawing_20250511.png</t>
@@ -9353,7 +9353,7 @@
         </is>
       </c>
     </row>
-    <row r="17">
+    <row r="17" ht="36" customHeight="1">
       <c r="B17" t="inlineStr">
         <is>
           <t>Schematic_countUD8L.png</t>
@@ -9365,7 +9365,7 @@
         </is>
       </c>
     </row>
-    <row r="18">
+    <row r="18" ht="94.5" customHeight="1">
       <c r="B18" t="inlineStr">
         <is>
           <t>Schematic_LFSR.png</t>
@@ -9377,7 +9377,7 @@
         </is>
       </c>
     </row>
-    <row r="19">
+    <row r="19" ht="23.25" customHeight="1">
       <c r="B19" t="inlineStr">
         <is>
           <t>Schematic_StateMachine4.png</t>
@@ -9389,7 +9389,7 @@
         </is>
       </c>
     </row>
-    <row r="20">
+    <row r="20" ht="38.25" customHeight="1">
       <c r="B20" t="inlineStr">
         <is>
           <t>Schematic_TopLevel4.png</t>
@@ -9401,7 +9401,7 @@
         </is>
       </c>
     </row>
-    <row r="21">
+    <row r="21" ht="46.5" customHeight="1">
       <c r="B21" t="inlineStr">
         <is>
           <t>Screenshot 2024-02-13 162201.png</t>
@@ -9413,7 +9413,7 @@
         </is>
       </c>
     </row>
-    <row r="22">
+    <row r="22" ht="46.5" customHeight="1">
       <c r="B22" t="inlineStr">
         <is>
           <t>Screenshot 2024-04-10 115750.png</t>
@@ -9425,7 +9425,7 @@
         </is>
       </c>
     </row>
-    <row r="23">
+    <row r="23" ht="43.5" customHeight="1">
       <c r="B23" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-05 181752.png</t>
@@ -9437,7 +9437,7 @@
         </is>
       </c>
     </row>
-    <row r="24">
+    <row r="24" ht="34.5" customHeight="1">
       <c r="B24" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-05 230541.png</t>
@@ -9449,7 +9449,7 @@
         </is>
       </c>
     </row>
-    <row r="25">
+    <row r="25" ht="46.5" customHeight="1">
       <c r="B25" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-06 212020.png</t>
@@ -9461,7 +9461,7 @@
         </is>
       </c>
     </row>
-    <row r="26">
+    <row r="26" ht="65.25" customHeight="1">
       <c r="B26" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-08 182509.png</t>
@@ -9473,7 +9473,7 @@
         </is>
       </c>
     </row>
-    <row r="27">
+    <row r="27" ht="192.75" customHeight="1">
       <c r="B27" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-11 003639.png</t>
@@ -9485,7 +9485,7 @@
         </is>
       </c>
     </row>
-    <row r="28">
+    <row r="28" ht="62.25" customHeight="1">
       <c r="B28" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-15 004329.png</t>
@@ -9497,7 +9497,7 @@
         </is>
       </c>
     </row>
-    <row r="29">
+    <row r="29" ht="61.5" customHeight="1">
       <c r="B29" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-15 004558.png</t>
@@ -9509,7 +9509,7 @@
         </is>
       </c>
     </row>
-    <row r="30">
+    <row r="30" ht="69" customHeight="1">
       <c r="B30" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-15 004709.png</t>
@@ -9521,7 +9521,7 @@
         </is>
       </c>
     </row>
-    <row r="31">
+    <row r="31" ht="69" customHeight="1">
       <c r="B31" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-15 005454.png</t>
@@ -9533,7 +9533,7 @@
         </is>
       </c>
     </row>
-    <row r="32">
+    <row r="32" ht="43.5" customHeight="1">
       <c r="B32" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-16 200955.png</t>
@@ -9545,7 +9545,7 @@
         </is>
       </c>
     </row>
-    <row r="33">
+    <row r="33" ht="46.5" customHeight="1">
       <c r="B33" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-16 204900.png</t>
@@ -9557,7 +9557,7 @@
         </is>
       </c>
     </row>
-    <row r="34">
+    <row r="34" ht="35.25" customHeight="1">
       <c r="B34" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-19 125316.png</t>
@@ -9569,7 +9569,7 @@
         </is>
       </c>
     </row>
-    <row r="35">
+    <row r="35" ht="50.25" customHeight="1">
       <c r="B35" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-20 163605.png</t>
@@ -9581,7 +9581,7 @@
         </is>
       </c>
     </row>
-    <row r="36">
+    <row r="36" ht="46.5" customHeight="1">
       <c r="B36" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-20 214348.png</t>
@@ -9593,7 +9593,7 @@
         </is>
       </c>
     </row>
-    <row r="37">
+    <row r="37" ht="42" customHeight="1">
       <c r="B37" t="inlineStr">
         <is>
           <t>Screenshot 2024-05-21 174330.png</t>
@@ -9605,7 +9605,7 @@
         </is>
       </c>
     </row>
-    <row r="38">
+    <row r="38" ht="15" customHeight="1">
       <c r="B38" t="inlineStr">
         <is>
           <t>Screenshot 2024-06-06 133307.png</t>
@@ -9617,7 +9617,7 @@
         </is>
       </c>
     </row>
-    <row r="39">
+    <row r="39" ht="15" customHeight="1">
       <c r="B39" t="inlineStr">
         <is>
           <t>Screenshot 2024-06-06 133440.png</t>
@@ -9629,7 +9629,7 @@
         </is>
       </c>
     </row>
-    <row r="40">
+    <row r="40" ht="46.5" customHeight="1">
       <c r="B40" t="inlineStr">
         <is>
           <t>Screenshot 2024-06-06 145654.png</t>
@@ -9641,7 +9641,7 @@
         </is>
       </c>
     </row>
-    <row r="41">
+    <row r="41" ht="44.25" customHeight="1">
       <c r="B41" t="inlineStr">
         <is>
           <t>Screenshot 2024-06-06 145713.png</t>
@@ -9653,7 +9653,7 @@
         </is>
       </c>
     </row>
-    <row r="42">
+    <row r="42" ht="46.5" customHeight="1">
       <c r="B42" t="inlineStr">
         <is>
           <t>Screenshot 2024-06-06 145822.png</t>
@@ -9665,7 +9665,7 @@
         </is>
       </c>
     </row>
-    <row r="43">
+    <row r="43" ht="44.25" customHeight="1">
       <c r="B43" t="inlineStr">
         <is>
           <t>Screenshot 2024-06-06 145840.png</t>
@@ -9677,7 +9677,7 @@
         </is>
       </c>
     </row>
-    <row r="44">
+    <row r="44" ht="46.5" customHeight="1">
       <c r="B44" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 172754.png</t>
@@ -9689,7 +9689,7 @@
         </is>
       </c>
     </row>
-    <row r="45">
+    <row r="45" ht="46.5" customHeight="1">
       <c r="B45" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 173050.png</t>
@@ -9701,7 +9701,7 @@
         </is>
       </c>
     </row>
-    <row r="46">
+    <row r="46" ht="46.5" customHeight="1">
       <c r="B46" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 173442.png</t>
@@ -9713,7 +9713,7 @@
         </is>
       </c>
     </row>
-    <row r="47">
+    <row r="47" ht="46.5" customHeight="1">
       <c r="B47" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 173452.png</t>
@@ -9725,7 +9725,7 @@
         </is>
       </c>
     </row>
-    <row r="48">
+    <row r="48" ht="46.5" customHeight="1">
       <c r="B48" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 173609.png</t>
@@ -9737,7 +9737,7 @@
         </is>
       </c>
     </row>
-    <row r="49">
+    <row r="49" ht="46.5" customHeight="1">
       <c r="B49" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 173648.png</t>
@@ -9749,7 +9749,7 @@
         </is>
       </c>
     </row>
-    <row r="50">
+    <row r="50" ht="46.5" customHeight="1">
       <c r="B50" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 173948.png</t>
@@ -9761,7 +9761,7 @@
         </is>
       </c>
     </row>
-    <row r="51">
+    <row r="51" ht="46.5" customHeight="1">
       <c r="B51" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 174301.png</t>
@@ -9773,7 +9773,7 @@
         </is>
       </c>
     </row>
-    <row r="52">
+    <row r="52" ht="46.5" customHeight="1">
       <c r="B52" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 174609.png</t>
@@ -9785,7 +9785,7 @@
         </is>
       </c>
     </row>
-    <row r="53">
+    <row r="53" ht="46.5" customHeight="1">
       <c r="B53" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 175019.png</t>
@@ -9797,7 +9797,7 @@
         </is>
       </c>
     </row>
-    <row r="54">
+    <row r="54" ht="46.5" customHeight="1">
       <c r="B54" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 175131.png</t>
@@ -9809,7 +9809,7 @@
         </is>
       </c>
     </row>
-    <row r="55">
+    <row r="55" ht="46.5" customHeight="1">
       <c r="B55" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 175330.png</t>
@@ -9821,7 +9821,7 @@
         </is>
       </c>
     </row>
-    <row r="56">
+    <row r="56" ht="46.5" customHeight="1">
       <c r="B56" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 175424.png</t>
@@ -9833,7 +9833,7 @@
         </is>
       </c>
     </row>
-    <row r="57">
+    <row r="57" ht="46.5" customHeight="1">
       <c r="B57" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 175531.png</t>
@@ -9845,7 +9845,7 @@
         </is>
       </c>
     </row>
-    <row r="58">
+    <row r="58" ht="46.5" customHeight="1">
       <c r="B58" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 175601.png</t>
@@ -9857,7 +9857,7 @@
         </is>
       </c>
     </row>
-    <row r="59">
+    <row r="59" ht="46.5" customHeight="1">
       <c r="B59" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 175650.png</t>
@@ -9869,7 +9869,7 @@
         </is>
       </c>
     </row>
-    <row r="60">
+    <row r="60" ht="46.5" customHeight="1">
       <c r="B60" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 175719.png</t>
@@ -9881,7 +9881,7 @@
         </is>
       </c>
     </row>
-    <row r="61">
+    <row r="61" ht="46.5" customHeight="1">
       <c r="B61" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 183259.png</t>
@@ -9893,7 +9893,7 @@
         </is>
       </c>
     </row>
-    <row r="62">
+    <row r="62" ht="46.5" customHeight="1">
       <c r="B62" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 183312.png</t>
@@ -9905,7 +9905,7 @@
         </is>
       </c>
     </row>
-    <row r="63">
+    <row r="63" ht="46.5" customHeight="1">
       <c r="B63" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-21 183357.png</t>
@@ -9917,7 +9917,7 @@
         </is>
       </c>
     </row>
-    <row r="64">
+    <row r="64" ht="46.5" customHeight="1">
       <c r="B64" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-23 120733.png</t>
@@ -9929,7 +9929,7 @@
         </is>
       </c>
     </row>
-    <row r="65">
+    <row r="65" ht="42" customHeight="1">
       <c r="B65" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-23 120856.png</t>
@@ -9941,7 +9941,7 @@
         </is>
       </c>
     </row>
-    <row r="66">
+    <row r="66" ht="69" customHeight="1">
       <c r="B66" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-23 121045.png</t>
@@ -9953,7 +9953,7 @@
         </is>
       </c>
     </row>
-    <row r="67">
+    <row r="67" ht="65.25" customHeight="1">
       <c r="B67" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-23 121751.png</t>
@@ -9965,7 +9965,7 @@
         </is>
       </c>
     </row>
-    <row r="68">
+    <row r="68" ht="73.5" customHeight="1">
       <c r="B68" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-23 121837.png</t>
@@ -9977,7 +9977,7 @@
         </is>
       </c>
     </row>
-    <row r="69">
+    <row r="69" ht="81" customHeight="1">
       <c r="B69" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-23 153432.png</t>
@@ -9989,7 +9989,7 @@
         </is>
       </c>
     </row>
-    <row r="70">
+    <row r="70" ht="21" customHeight="1">
       <c r="B70" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-23 153506.png</t>
@@ -10001,7 +10001,7 @@
         </is>
       </c>
     </row>
-    <row r="71">
+    <row r="71" ht="26.25" customHeight="1">
       <c r="B71" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-23 153608.png</t>
@@ -10013,7 +10013,7 @@
         </is>
       </c>
     </row>
-    <row r="72">
+    <row r="72" ht="66.75" customHeight="1">
       <c r="B72" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-23 154559.png</t>
@@ -10025,7 +10025,7 @@
         </is>
       </c>
     </row>
-    <row r="73">
+    <row r="73" ht="78.75" customHeight="1">
       <c r="B73" t="inlineStr">
         <is>
           <t>Screenshot 2024-08-23 155425.png</t>
@@ -10037,7 +10037,7 @@
         </is>
       </c>
     </row>
-    <row r="74">
+    <row r="74" ht="55.5" customHeight="1">
       <c r="B74" t="inlineStr">
         <is>
           <t>Screenshot 2024-09-20 091542.png</t>
@@ -10049,7 +10049,7 @@
         </is>
       </c>
     </row>
-    <row r="75">
+    <row r="75" ht="46.5" customHeight="1">
       <c r="B75" t="inlineStr">
         <is>
           <t>Screenshot 2024-09-22 114109.png</t>
@@ -10061,7 +10061,7 @@
         </is>
       </c>
     </row>
-    <row r="76">
+    <row r="76" ht="46.5" customHeight="1">
       <c r="B76" t="inlineStr">
         <is>
           <t>Screenshot 2024-09-22 142408.png</t>
@@ -10073,7 +10073,7 @@
         </is>
       </c>
     </row>
-    <row r="77">
+    <row r="77" ht="46.5" customHeight="1">
       <c r="B77" t="inlineStr">
         <is>
           <t>Screenshot 2024-09-22 145507.png</t>
@@ -10085,7 +10085,7 @@
         </is>
       </c>
     </row>
-    <row r="78">
+    <row r="78" ht="46.5" customHeight="1">
       <c r="B78" t="inlineStr">
         <is>
           <t>Screenshot 2024-09-26 220350.png</t>
@@ -10097,7 +10097,7 @@
         </is>
       </c>
     </row>
-    <row r="79">
+    <row r="79" ht="39.75" customHeight="1">
       <c r="B79" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-03 135514.png</t>
@@ -10109,7 +10109,7 @@
         </is>
       </c>
     </row>
-    <row r="80">
+    <row r="80" ht="42.75" customHeight="1">
       <c r="B80" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-04 023958.png</t>
@@ -10121,7 +10121,7 @@
         </is>
       </c>
     </row>
-    <row r="81">
+    <row r="81" ht="72" customHeight="1">
       <c r="B81" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-04 115639.png</t>
@@ -10133,7 +10133,7 @@
         </is>
       </c>
     </row>
-    <row r="82">
+    <row r="82" ht="105" customHeight="1">
       <c r="B82" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-04 211319.png</t>
@@ -10145,7 +10145,7 @@
         </is>
       </c>
     </row>
-    <row r="83">
+    <row r="83" ht="103.5" customHeight="1">
       <c r="B83" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-04 212457.png</t>
@@ -10157,7 +10157,7 @@
         </is>
       </c>
     </row>
-    <row r="84">
+    <row r="84" ht="125.25" customHeight="1">
       <c r="B84" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-04 222748.png</t>
@@ -10169,7 +10169,7 @@
         </is>
       </c>
     </row>
-    <row r="85">
+    <row r="85" ht="133.5" customHeight="1">
       <c r="B85" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-04 224728.png</t>
@@ -10181,7 +10181,7 @@
         </is>
       </c>
     </row>
-    <row r="86">
+    <row r="86" ht="38.25" customHeight="1">
       <c r="B86" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-06 163417.png</t>
@@ -10193,7 +10193,7 @@
         </is>
       </c>
     </row>
-    <row r="87">
+    <row r="87" ht="81" customHeight="1">
       <c r="B87" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-14 105051.png</t>
@@ -10205,7 +10205,7 @@
         </is>
       </c>
     </row>
-    <row r="88">
+    <row r="88" ht="45" customHeight="1">
       <c r="B88" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-15 141604.png</t>
@@ -10217,7 +10217,7 @@
         </is>
       </c>
     </row>
-    <row r="89">
+    <row r="89" ht="21" customHeight="1">
       <c r="B89" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-24 123911.png</t>
@@ -10229,7 +10229,7 @@
         </is>
       </c>
     </row>
-    <row r="90">
+    <row r="90" ht="62.25" customHeight="1">
       <c r="B90" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-24 223327.png</t>
@@ -10241,7 +10241,7 @@
         </is>
       </c>
     </row>
-    <row r="91">
+    <row r="91" ht="33" customHeight="1">
       <c r="B91" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-25 170451.png</t>
@@ -10253,7 +10253,7 @@
         </is>
       </c>
     </row>
-    <row r="92">
+    <row r="92" ht="46.5" customHeight="1">
       <c r="B92" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-26 220604.png</t>
@@ -10265,7 +10265,7 @@
         </is>
       </c>
     </row>
-    <row r="93">
+    <row r="93" ht="46.5" customHeight="1">
       <c r="B93" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-26 220800.png</t>
@@ -10277,7 +10277,7 @@
         </is>
       </c>
     </row>
-    <row r="94">
+    <row r="94" ht="63" customHeight="1">
       <c r="B94" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-27 194648.png</t>
@@ -10289,7 +10289,7 @@
         </is>
       </c>
     </row>
-    <row r="95">
+    <row r="95" ht="90" customHeight="1">
       <c r="B95" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-27 194741.png</t>
@@ -10301,7 +10301,7 @@
         </is>
       </c>
     </row>
-    <row r="96">
+    <row r="96" ht="75.75" customHeight="1">
       <c r="B96" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-27 194822.png</t>
@@ -10313,7 +10313,7 @@
         </is>
       </c>
     </row>
-    <row r="97">
+    <row r="97" ht="51" customHeight="1">
       <c r="B97" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-29 222129.png</t>
@@ -10325,7 +10325,7 @@
         </is>
       </c>
     </row>
-    <row r="98">
+    <row r="98" ht="55.5" customHeight="1">
       <c r="B98" t="inlineStr">
         <is>
           <t>Screenshot 2024-10-29 224435.png</t>
@@ -10337,7 +10337,7 @@
         </is>
       </c>
     </row>
-    <row r="99">
+    <row r="99" ht="41.25" customHeight="1">
       <c r="B99" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 123302.png</t>
@@ -10349,7 +10349,7 @@
         </is>
       </c>
     </row>
-    <row r="100">
+    <row r="100" ht="75.75" customHeight="1">
       <c r="B100" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 124348.png</t>
@@ -10361,7 +10361,7 @@
         </is>
       </c>
     </row>
-    <row r="101">
+    <row r="101" ht="50.25" customHeight="1">
       <c r="B101" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 124852.png</t>
@@ -10373,7 +10373,7 @@
         </is>
       </c>
     </row>
-    <row r="102">
+    <row r="102" ht="69" customHeight="1">
       <c r="B102" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 130607.png</t>
@@ -10385,7 +10385,7 @@
         </is>
       </c>
     </row>
-    <row r="103">
+    <row r="103" ht="54" customHeight="1">
       <c r="B103" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 131444.png</t>
@@ -10397,7 +10397,7 @@
         </is>
       </c>
     </row>
-    <row r="104">
+    <row r="104" ht="39.75" customHeight="1">
       <c r="B104" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 131828.png</t>
@@ -10409,7 +10409,7 @@
         </is>
       </c>
     </row>
-    <row r="105">
+    <row r="105" ht="45" customHeight="1">
       <c r="B105" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 154227.png</t>
@@ -10421,7 +10421,7 @@
         </is>
       </c>
     </row>
-    <row r="106">
+    <row r="106" ht="57" customHeight="1">
       <c r="B106" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 165110.png</t>
@@ -10433,7 +10433,7 @@
         </is>
       </c>
     </row>
-    <row r="107">
+    <row r="107" ht="50.25" customHeight="1">
       <c r="B107" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 170428.png</t>
@@ -10445,7 +10445,7 @@
         </is>
       </c>
     </row>
-    <row r="108">
+    <row r="108" ht="34.5" customHeight="1">
       <c r="B108" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 191934.png</t>
@@ -10457,7 +10457,7 @@
         </is>
       </c>
     </row>
-    <row r="109">
+    <row r="109" ht="35.25" customHeight="1">
       <c r="B109" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 192257.png</t>
@@ -10469,7 +10469,7 @@
         </is>
       </c>
     </row>
-    <row r="110">
+    <row r="110" ht="46.5" customHeight="1">
       <c r="B110" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 193111.png</t>
@@ -10481,7 +10481,7 @@
         </is>
       </c>
     </row>
-    <row r="111">
+    <row r="111" ht="94.5" customHeight="1">
       <c r="B111" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 193139.png</t>
@@ -10493,7 +10493,7 @@
         </is>
       </c>
     </row>
-    <row r="112">
+    <row r="112" ht="6.75" customHeight="1">
       <c r="B112" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-03 193537.png</t>
@@ -10505,7 +10505,7 @@
         </is>
       </c>
     </row>
-    <row r="113">
+    <row r="113" ht="51.75" customHeight="1">
       <c r="B113" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-04 152138.png</t>
@@ -10517,7 +10517,7 @@
         </is>
       </c>
     </row>
-    <row r="114">
+    <row r="114" ht="59.25" customHeight="1">
       <c r="B114" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-04 153823.png</t>
@@ -10529,7 +10529,7 @@
         </is>
       </c>
     </row>
-    <row r="115">
+    <row r="115" ht="41.25" customHeight="1">
       <c r="B115" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-04 155152.png</t>
@@ -10541,7 +10541,7 @@
         </is>
       </c>
     </row>
-    <row r="116">
+    <row r="116" ht="48" customHeight="1">
       <c r="B116" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-05 191357.png</t>
@@ -10553,7 +10553,7 @@
         </is>
       </c>
     </row>
-    <row r="117">
+    <row r="117" ht="48.75" customHeight="1">
       <c r="B117" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-05 191452.png</t>
@@ -10565,7 +10565,7 @@
         </is>
       </c>
     </row>
-    <row r="118">
+    <row r="118" ht="13.5" customHeight="1">
       <c r="B118" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-05 223636.png</t>
@@ -10577,7 +10577,7 @@
         </is>
       </c>
     </row>
-    <row r="119">
+    <row r="119" ht="80.25" customHeight="1">
       <c r="B119" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-06 011018.png</t>
@@ -10589,7 +10589,7 @@
         </is>
       </c>
     </row>
-    <row r="120">
+    <row r="120" ht="63.75" customHeight="1">
       <c r="B120" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-06 015530.png</t>
@@ -10601,7 +10601,7 @@
         </is>
       </c>
     </row>
-    <row r="121">
+    <row r="121" ht="20.25" customHeight="1">
       <c r="B121" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-10 015738.png</t>
@@ -10613,7 +10613,7 @@
         </is>
       </c>
     </row>
-    <row r="122">
+    <row r="122" ht="39" customHeight="1">
       <c r="B122" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-10 045303.png</t>
@@ -10625,7 +10625,7 @@
         </is>
       </c>
     </row>
-    <row r="123">
+    <row r="123" ht="36" customHeight="1">
       <c r="B123" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-10 045401.png</t>
@@ -10637,7 +10637,7 @@
         </is>
       </c>
     </row>
-    <row r="124">
+    <row r="124" ht="46.5" customHeight="1">
       <c r="B124" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-10 050351.png</t>
@@ -10649,7 +10649,7 @@
         </is>
       </c>
     </row>
-    <row r="125">
+    <row r="125" ht="46.5" customHeight="1">
       <c r="B125" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-10 050525.png</t>
@@ -10661,7 +10661,7 @@
         </is>
       </c>
     </row>
-    <row r="126">
+    <row r="126" ht="21" customHeight="1">
       <c r="B126" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-10 050615 - Copy.png</t>
@@ -10673,7 +10673,7 @@
         </is>
       </c>
     </row>
-    <row r="127">
+    <row r="127" ht="46.5" customHeight="1">
       <c r="B127" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-10 050615.png</t>
@@ -10685,7 +10685,7 @@
         </is>
       </c>
     </row>
-    <row r="128">
+    <row r="128" ht="46.5" customHeight="1">
       <c r="B128" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-10 221231.png</t>
@@ -10697,7 +10697,7 @@
         </is>
       </c>
     </row>
-    <row r="129">
+    <row r="129" ht="46.5" customHeight="1">
       <c r="B129" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-13 002332.png</t>
@@ -10709,7 +10709,7 @@
         </is>
       </c>
     </row>
-    <row r="130">
+    <row r="130" ht="46.5" customHeight="1">
       <c r="B130" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-15 005845.png</t>
@@ -10721,7 +10721,7 @@
         </is>
       </c>
     </row>
-    <row r="131">
+    <row r="131" ht="38.25" customHeight="1">
       <c r="B131" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-15 005912.png</t>
@@ -10733,7 +10733,7 @@
         </is>
       </c>
     </row>
-    <row r="132">
+    <row r="132" ht="39.75" customHeight="1">
       <c r="B132" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-15 164035.png</t>
@@ -10745,7 +10745,7 @@
         </is>
       </c>
     </row>
-    <row r="133">
+    <row r="133" ht="28.5" customHeight="1">
       <c r="B133" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-16 182546.png</t>
@@ -10757,7 +10757,7 @@
         </is>
       </c>
     </row>
-    <row r="134">
+    <row r="134" ht="46.5" customHeight="1">
       <c r="B134" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-16 225139.png</t>
@@ -10769,7 +10769,7 @@
         </is>
       </c>
     </row>
-    <row r="135">
+    <row r="135" ht="46.5" customHeight="1">
       <c r="B135" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-16 225306.png</t>
@@ -10781,7 +10781,7 @@
         </is>
       </c>
     </row>
-    <row r="136">
+    <row r="136" ht="46.5" customHeight="1">
       <c r="B136" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-16 230722.png</t>
@@ -10793,7 +10793,7 @@
         </is>
       </c>
     </row>
-    <row r="137">
+    <row r="137" ht="46.5" customHeight="1">
       <c r="B137" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-16 230841.png</t>
@@ -10805,7 +10805,7 @@
         </is>
       </c>
     </row>
-    <row r="138">
+    <row r="138" ht="46.5" customHeight="1">
       <c r="B138" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-16 230947.png</t>
@@ -10817,7 +10817,7 @@
         </is>
       </c>
     </row>
-    <row r="139">
+    <row r="139" ht="46.5" customHeight="1">
       <c r="B139" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-16 232103.png</t>
@@ -10829,7 +10829,7 @@
         </is>
       </c>
     </row>
-    <row r="140">
+    <row r="140" ht="46.5" customHeight="1">
       <c r="B140" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-16 232851.png</t>
@@ -10841,7 +10841,7 @@
         </is>
       </c>
     </row>
-    <row r="141">
+    <row r="141" ht="46.5" customHeight="1">
       <c r="B141" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-17 010536.png</t>
@@ -10853,7 +10853,7 @@
         </is>
       </c>
     </row>
-    <row r="142">
+    <row r="142" ht="46.5" customHeight="1">
       <c r="B142" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-17 014109.png</t>
@@ -10865,7 +10865,7 @@
         </is>
       </c>
     </row>
-    <row r="143">
+    <row r="143" ht="46.5" customHeight="1">
       <c r="B143" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-18 152149.png</t>
@@ -10877,7 +10877,7 @@
         </is>
       </c>
     </row>
-    <row r="144">
+    <row r="144" ht="46.5" customHeight="1">
       <c r="B144" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-18 154311.png</t>
@@ -10889,7 +10889,7 @@
         </is>
       </c>
     </row>
-    <row r="145">
+    <row r="145" ht="46.5" customHeight="1">
       <c r="B145" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-18 160328.png</t>
@@ -10901,7 +10901,7 @@
         </is>
       </c>
     </row>
-    <row r="146">
+    <row r="146" ht="46.5" customHeight="1">
       <c r="B146" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-18 164815.png</t>
@@ -10913,7 +10913,7 @@
         </is>
       </c>
     </row>
-    <row r="147">
+    <row r="147" ht="46.5" customHeight="1">
       <c r="B147" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-28 194603.png</t>
@@ -10925,7 +10925,7 @@
         </is>
       </c>
     </row>
-    <row r="148">
+    <row r="148" ht="38.25" customHeight="1">
       <c r="B148" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-28 194628.png</t>
@@ -10937,7 +10937,7 @@
         </is>
       </c>
     </row>
-    <row r="149">
+    <row r="149" ht="90" customHeight="1">
       <c r="B149" t="inlineStr">
         <is>
           <t>Screenshot 2024-11-30 173310.png</t>
@@ -10949,7 +10949,7 @@
         </is>
       </c>
     </row>
-    <row r="150">
+    <row r="150" ht="60.75" customHeight="1">
       <c r="B150" t="inlineStr">
         <is>
           <t>Screenshot 2024-12-06 160548.png</t>
@@ -10961,7 +10961,7 @@
         </is>
       </c>
     </row>
-    <row r="151">
+    <row r="151" ht="31.5" customHeight="1">
       <c r="B151" t="inlineStr">
         <is>
           <t>Screenshot 2024-12-13 122228.png</t>
@@ -10973,7 +10973,7 @@
         </is>
       </c>
     </row>
-    <row r="152">
+    <row r="152" ht="39" customHeight="1">
       <c r="B152" t="inlineStr">
         <is>
           <t>Screenshot 2024-12-13 132924.png</t>
@@ -10985,7 +10985,7 @@
         </is>
       </c>
     </row>
-    <row r="153">
+    <row r="153" ht="46.5" customHeight="1">
       <c r="B153" t="inlineStr">
         <is>
           <t>Screenshot 2024-12-13 142435.png</t>
@@ -10997,7 +10997,7 @@
         </is>
       </c>
     </row>
-    <row r="154">
+    <row r="154" ht="69" customHeight="1">
       <c r="B154" t="inlineStr">
         <is>
           <t>Screenshot 2024-12-13 142454.png</t>
@@ -11009,7 +11009,7 @@
         </is>
       </c>
     </row>
-    <row r="155">
+    <row r="155" ht="48.75" customHeight="1">
       <c r="B155" t="inlineStr">
         <is>
           <t>Screenshot 2024-12-13 145322.png</t>
@@ -11021,7 +11021,7 @@
         </is>
       </c>
     </row>
-    <row r="156">
+    <row r="156" ht="24.75" customHeight="1">
       <c r="B156" t="inlineStr">
         <is>
           <t>Screenshot 2024-12-13 153654.png</t>
@@ -11033,7 +11033,7 @@
         </is>
       </c>
     </row>
-    <row r="157">
+    <row r="157" ht="82.5" customHeight="1">
       <c r="B157" t="inlineStr">
         <is>
           <t>Screenshot 2024-12-13 155304.png</t>
@@ -11045,7 +11045,7 @@
         </is>
       </c>
     </row>
-    <row r="158">
+    <row r="158" ht="72.75" customHeight="1">
       <c r="B158" t="inlineStr">
         <is>
           <t>Screenshot 2024-12-19 212609.png</t>
@@ -11057,7 +11057,7 @@
         </is>
       </c>
     </row>
-    <row r="159">
+    <row r="159" ht="65.25" customHeight="1">
       <c r="B159" t="inlineStr">
         <is>
           <t>Screenshot 2024-12-30 121431.png</t>
@@ -11069,7 +11069,7 @@
         </is>
       </c>
     </row>
-    <row r="160">
+    <row r="160" ht="112.5" customHeight="1">
       <c r="B160" t="inlineStr">
         <is>
           <t>Screenshot 2024-12-31 105754.png</t>
@@ -11081,7 +11081,7 @@
         </is>
       </c>
     </row>
-    <row r="161">
+    <row r="161" ht="77.25" customHeight="1">
       <c r="B161" t="inlineStr">
         <is>
           <t>Screenshot 2024-12-31 105829.png</t>
@@ -11093,7 +11093,7 @@
         </is>
       </c>
     </row>
-    <row r="162">
+    <row r="162" ht="16.5" customHeight="1">
       <c r="B162" t="inlineStr">
         <is>
           <t>Screenshot 2024-12-31 171125.png</t>
@@ -11105,7 +11105,7 @@
         </is>
       </c>
     </row>
-    <row r="163">
+    <row r="163" ht="48.75" customHeight="1">
       <c r="B163" t="inlineStr">
         <is>
           <t>Screenshot 2025-01-04 204209.png</t>
@@ -11117,7 +11117,7 @@
         </is>
       </c>
     </row>
-    <row r="164">
+    <row r="164" ht="57" customHeight="1">
       <c r="B164" t="inlineStr">
         <is>
           <t>Screenshot 2025-01-06 130545.png</t>
@@ -11129,7 +11129,7 @@
         </is>
       </c>
     </row>
-    <row r="165">
+    <row r="165" ht="39.75" customHeight="1">
       <c r="B165" t="inlineStr">
         <is>
           <t>Screenshot 2025-01-08 104701.png</t>
@@ -11141,7 +11141,7 @@
         </is>
       </c>
     </row>
-    <row r="166">
+    <row r="166" ht="24" customHeight="1">
       <c r="B166" t="inlineStr">
         <is>
           <t>Screenshot 2025-01-09 193717.png</t>
@@ -11153,7 +11153,7 @@
         </is>
       </c>
     </row>
-    <row r="167">
+    <row r="167" ht="25.5" customHeight="1">
       <c r="B167" t="inlineStr">
         <is>
           <t>Screenshot 2025-01-10 103319.png</t>
@@ -11165,7 +11165,7 @@
         </is>
       </c>
     </row>
-    <row r="168">
+    <row r="168" ht="81" customHeight="1">
       <c r="B168" t="inlineStr">
         <is>
           <t>Screenshot 2025-01-13 092258.png</t>
@@ -11177,7 +11177,7 @@
         </is>
       </c>
     </row>
-    <row r="169">
+    <row r="169" ht="40.5" customHeight="1">
       <c r="B169" t="inlineStr">
         <is>
           <t>Screenshot 2025-01-14 191957.png</t>
@@ -11189,7 +11189,7 @@
         </is>
       </c>
     </row>
-    <row r="170">
+    <row r="170" ht="42" customHeight="1">
       <c r="B170" t="inlineStr">
         <is>
           <t>Screenshot 2025-01-25 1637221.png</t>
@@ -11201,7 +11201,7 @@
         </is>
       </c>
     </row>
-    <row r="171">
+    <row r="171" ht="46.5" customHeight="1">
       <c r="B171" t="inlineStr">
         <is>
           <t>Screenshot 2025-01-26 192143.png</t>
@@ -11213,7 +11213,7 @@
         </is>
       </c>
     </row>
-    <row r="172">
+    <row r="172" ht="42" customHeight="1">
       <c r="B172" t="inlineStr">
         <is>
           <t>Screenshot 2025-01-27 2020.png</t>
@@ -11225,7 +11225,7 @@
         </is>
       </c>
     </row>
-    <row r="173">
+    <row r="173" ht="42.75" customHeight="1">
       <c r="B173" t="inlineStr">
         <is>
           <t>Screenshot 2025-01-30 163427.png</t>
@@ -11237,7 +11237,7 @@
         </is>
       </c>
     </row>
-    <row r="174">
+    <row r="174" ht="45.75" customHeight="1">
       <c r="B174" t="inlineStr">
         <is>
           <t>Screenshot 2025-02-01 154745.png</t>
@@ -11249,7 +11249,7 @@
         </is>
       </c>
     </row>
-    <row r="175">
+    <row r="175" ht="45.75" customHeight="1">
       <c r="B175" t="inlineStr">
         <is>
           <t>Screenshot 2025-02-01 164250.png</t>
@@ -11261,7 +11261,7 @@
         </is>
       </c>
     </row>
-    <row r="176">
+    <row r="176" ht="68.25" customHeight="1">
       <c r="B176" t="inlineStr">
         <is>
           <t>Screenshot 2025-02-01 175456.png</t>
@@ -11273,7 +11273,7 @@
         </is>
       </c>
     </row>
-    <row r="177">
+    <row r="177" ht="12" customHeight="1">
       <c r="B177" t="inlineStr">
         <is>
           <t>Screenshot 2025-02-02 103645.png</t>
@@ -11285,7 +11285,7 @@
         </is>
       </c>
     </row>
-    <row r="178">
+    <row r="178" ht="42.75" customHeight="1">
       <c r="B178" t="inlineStr">
         <is>
           <t>Screenshot 2025-02-12 094704.png</t>
@@ -11297,7 +11297,7 @@
         </is>
       </c>
     </row>
-    <row r="179">
+    <row r="179" ht="41.25" customHeight="1">
       <c r="B179" t="inlineStr">
         <is>
           <t>Screenshot 2025-02-12 094928.png</t>
@@ -11309,7 +11309,7 @@
         </is>
       </c>
     </row>
-    <row r="180">
+    <row r="180" ht="41.25" customHeight="1">
       <c r="B180" t="inlineStr">
         <is>
           <t>Screenshot 2025-02-12 095450.png</t>
@@ -11321,7 +11321,7 @@
         </is>
       </c>
     </row>
-    <row r="181">
+    <row r="181" ht="41.25" customHeight="1">
       <c r="B181" t="inlineStr">
         <is>
           <t>Screenshot 2025-02-12 100041.png</t>
@@ -11333,7 +11333,7 @@
         </is>
       </c>
     </row>
-    <row r="182">
+    <row r="182" ht="42" customHeight="1">
       <c r="B182" t="inlineStr">
         <is>
           <t>Screenshot 2025-02-21 105333.png</t>
@@ -11345,7 +11345,7 @@
         </is>
       </c>
     </row>
-    <row r="183">
+    <row r="183" ht="99" customHeight="1">
       <c r="B183" t="inlineStr">
         <is>
           <t>Screenshot 2025-03-01 111629.png</t>
@@ -11357,7 +11357,7 @@
         </is>
       </c>
     </row>
-    <row r="184">
+    <row r="184" ht="45.75" customHeight="1">
       <c r="B184" t="inlineStr">
         <is>
           <t>Screenshot 2025-03-04 120746.png</t>
@@ -11369,7 +11369,7 @@
         </is>
       </c>
     </row>
-    <row r="185">
+    <row r="185" ht="44.25" customHeight="1">
       <c r="B185" t="inlineStr">
         <is>
           <t>Screenshot 2025-03-06 130350.png</t>
@@ -11381,7 +11381,7 @@
         </is>
       </c>
     </row>
-    <row r="186">
+    <row r="186" ht="14.25" customHeight="1">
       <c r="B186" t="inlineStr">
         <is>
           <t>Screenshot 2025-03-07 114625.png</t>
@@ -11393,7 +11393,7 @@
         </is>
       </c>
     </row>
-    <row r="187">
+    <row r="187" ht="14.25" customHeight="1">
       <c r="B187" t="inlineStr">
         <is>
           <t>Screenshot 2025-03-07 114732.png</t>
@@ -11405,7 +11405,7 @@
         </is>
       </c>
     </row>
-    <row r="188">
+    <row r="188" ht="45" customHeight="1">
       <c r="B188" t="inlineStr">
         <is>
           <t>Screenshot 2025-03-07 120723.png</t>
@@ -11417,7 +11417,7 @@
         </is>
       </c>
     </row>
-    <row r="189">
+    <row r="189" ht="66" customHeight="1">
       <c r="B189" t="inlineStr">
         <is>
           <t>Screenshot 2025-03-10 135413.png</t>
@@ -11429,7 +11429,7 @@
         </is>
       </c>
     </row>
-    <row r="190">
+    <row r="190" ht="54.75" customHeight="1">
       <c r="B190" t="inlineStr">
         <is>
           <t>Screenshot 2025-03-17 175519.png</t>
@@ -11441,7 +11441,7 @@
         </is>
       </c>
     </row>
-    <row r="191">
+    <row r="191" ht="46.5" customHeight="1">
       <c r="B191" t="inlineStr">
         <is>
           <t>Screenshot 2025-03-25 144731.png</t>
@@ -11453,7 +11453,7 @@
         </is>
       </c>
     </row>
-    <row r="192">
+    <row r="192" ht="59.25" customHeight="1">
       <c r="B192" t="inlineStr">
         <is>
           <t>Screenshot 2025-03-30 225813.png</t>
@@ -11465,7 +11465,7 @@
         </is>
       </c>
     </row>
-    <row r="193">
+    <row r="193" ht="44.25" customHeight="1">
       <c r="B193" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-02 144720.png</t>
@@ -11477,7 +11477,7 @@
         </is>
       </c>
     </row>
-    <row r="194">
+    <row r="194" ht="41.25" customHeight="1">
       <c r="B194" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-03 120846.png</t>
@@ -11489,7 +11489,7 @@
         </is>
       </c>
     </row>
-    <row r="195">
+    <row r="195" ht="86.25" customHeight="1">
       <c r="B195" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-03 121759.png</t>
@@ -11501,7 +11501,7 @@
         </is>
       </c>
     </row>
-    <row r="196">
+    <row r="196" ht="20.25" customHeight="1">
       <c r="B196" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-03 124852.png</t>
@@ -11513,7 +11513,7 @@
         </is>
       </c>
     </row>
-    <row r="197">
+    <row r="197" ht="46.5" customHeight="1">
       <c r="B197" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-06 130427.png</t>
@@ -11525,7 +11525,7 @@
         </is>
       </c>
     </row>
-    <row r="198">
+    <row r="198" ht="21" customHeight="1">
       <c r="B198" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-06 191326.png</t>
@@ -11537,7 +11537,7 @@
         </is>
       </c>
     </row>
-    <row r="199">
+    <row r="199" ht="33.75" customHeight="1">
       <c r="B199" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-09 103507.png</t>
@@ -11549,7 +11549,7 @@
         </is>
       </c>
     </row>
-    <row r="200">
+    <row r="200" ht="33.75" customHeight="1">
       <c r="B200" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-11 173313.png</t>
@@ -11561,7 +11561,7 @@
         </is>
       </c>
     </row>
-    <row r="201">
+    <row r="201" ht="31.5" customHeight="1">
       <c r="B201" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-12 102301.png</t>
@@ -11573,7 +11573,7 @@
         </is>
       </c>
     </row>
-    <row r="202">
+    <row r="202" ht="48" customHeight="1">
       <c r="B202" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-12 160155.png</t>
@@ -11585,7 +11585,7 @@
         </is>
       </c>
     </row>
-    <row r="203">
+    <row r="203" ht="62.25" customHeight="1">
       <c r="B203" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-12 163247.png</t>
@@ -11597,7 +11597,7 @@
         </is>
       </c>
     </row>
-    <row r="204">
+    <row r="204" ht="39" customHeight="1">
       <c r="B204" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-12 164726.png</t>
@@ -11609,7 +11609,7 @@
         </is>
       </c>
     </row>
-    <row r="205">
+    <row r="205" ht="17.25" customHeight="1">
       <c r="B205" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-12 164812.png</t>
@@ -11621,7 +11621,7 @@
         </is>
       </c>
     </row>
-    <row r="206">
+    <row r="206" ht="37.5" customHeight="1">
       <c r="B206" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-12 165408.png</t>
@@ -11633,7 +11633,7 @@
         </is>
       </c>
     </row>
-    <row r="207">
+    <row r="207" ht="17.25" customHeight="1">
       <c r="B207" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-12 165552.png</t>
@@ -11645,7 +11645,7 @@
         </is>
       </c>
     </row>
-    <row r="208">
+    <row r="208" ht="17.25" customHeight="1">
       <c r="B208" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-12 170200.png</t>
@@ -11657,7 +11657,7 @@
         </is>
       </c>
     </row>
-    <row r="209">
+    <row r="209" ht="38.25" customHeight="1">
       <c r="B209" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-12 170250.png</t>
@@ -11669,7 +11669,7 @@
         </is>
       </c>
     </row>
-    <row r="210">
+    <row r="210" ht="40.5" customHeight="1">
       <c r="B210" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-12 171705.png</t>
@@ -11681,7 +11681,7 @@
         </is>
       </c>
     </row>
-    <row r="211">
+    <row r="211" ht="46.5" customHeight="1">
       <c r="B211" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-15 095113.png</t>
@@ -11693,7 +11693,7 @@
         </is>
       </c>
     </row>
-    <row r="212">
+    <row r="212" ht="46.5" customHeight="1">
       <c r="B212" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-16 124546.png</t>
@@ -11705,7 +11705,7 @@
         </is>
       </c>
     </row>
-    <row r="213">
+    <row r="213" ht="93" customHeight="1">
       <c r="B213" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-17 163602.png</t>
@@ -11717,7 +11717,7 @@
         </is>
       </c>
     </row>
-    <row r="214">
+    <row r="214" ht="92.25" customHeight="1">
       <c r="B214" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-17 163650.png</t>
@@ -11729,7 +11729,7 @@
         </is>
       </c>
     </row>
-    <row r="215">
+    <row r="215" ht="92.25" customHeight="1">
       <c r="B215" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-17 164424.png</t>
@@ -11741,7 +11741,7 @@
         </is>
       </c>
     </row>
-    <row r="216">
+    <row r="216" ht="93" customHeight="1">
       <c r="B216" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-17 164549.png</t>
@@ -11753,7 +11753,7 @@
         </is>
       </c>
     </row>
-    <row r="217">
+    <row r="217" ht="93" customHeight="1">
       <c r="B217" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-17 164719.png</t>
@@ -11765,7 +11765,7 @@
         </is>
       </c>
     </row>
-    <row r="218">
+    <row r="218" ht="93" customHeight="1">
       <c r="B218" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-17 164859.png</t>
@@ -11777,7 +11777,7 @@
         </is>
       </c>
     </row>
-    <row r="219">
+    <row r="219" ht="92.25" customHeight="1">
       <c r="B219" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-17 165109.png</t>
@@ -11789,7 +11789,7 @@
         </is>
       </c>
     </row>
-    <row r="220">
+    <row r="220" ht="80.25" customHeight="1">
       <c r="B220" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-17 172108.png</t>
@@ -11801,7 +11801,7 @@
         </is>
       </c>
     </row>
-    <row r="221">
+    <row r="221" ht="127.5" customHeight="1">
       <c r="B221" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-17 172143.png</t>
@@ -11813,7 +11813,7 @@
         </is>
       </c>
     </row>
-    <row r="222">
+    <row r="222" ht="46.5" customHeight="1">
       <c r="B222" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-19 205907.png</t>
@@ -11825,7 +11825,7 @@
         </is>
       </c>
     </row>
-    <row r="223">
+    <row r="223" ht="40.5" customHeight="1">
       <c r="B223" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-21 194344.png</t>
@@ -11837,7 +11837,7 @@
         </is>
       </c>
     </row>
-    <row r="224">
+    <row r="224" ht="46.5" customHeight="1">
       <c r="B224" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-21 194424.png</t>
@@ -11849,7 +11849,7 @@
         </is>
       </c>
     </row>
-    <row r="225">
+    <row r="225" ht="46.5" customHeight="1">
       <c r="B225" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-21 194655.png</t>
@@ -11861,7 +11861,7 @@
         </is>
       </c>
     </row>
-    <row r="226">
+    <row r="226" ht="46.5" customHeight="1">
       <c r="B226" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-21 194812.png</t>
@@ -11873,7 +11873,7 @@
         </is>
       </c>
     </row>
-    <row r="227">
+    <row r="227" ht="46.5" customHeight="1">
       <c r="B227" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-21 194951.png</t>
@@ -11885,7 +11885,7 @@
         </is>
       </c>
     </row>
-    <row r="228">
+    <row r="228" ht="46.5" customHeight="1">
       <c r="B228" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-21 195024.png</t>
@@ -11897,7 +11897,7 @@
         </is>
       </c>
     </row>
-    <row r="229">
+    <row r="229" ht="93" customHeight="1">
       <c r="B229" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-21 collage.png</t>
@@ -11909,7 +11909,7 @@
         </is>
       </c>
     </row>
-    <row r="230">
+    <row r="230" ht="46.5" customHeight="1">
       <c r="B230" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-22 081328.png</t>
@@ -11921,7 +11921,7 @@
         </is>
       </c>
     </row>
-    <row r="231">
+    <row r="231" ht="46.5" customHeight="1">
       <c r="B231" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-24 212857.png</t>
@@ -11933,7 +11933,7 @@
         </is>
       </c>
     </row>
-    <row r="232">
+    <row r="232" ht="46.5" customHeight="1">
       <c r="B232" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-24 213203.png</t>
@@ -11945,7 +11945,7 @@
         </is>
       </c>
     </row>
-    <row r="233">
+    <row r="233" ht="46.5" customHeight="1">
       <c r="B233" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-24 213230.png</t>
@@ -11957,7 +11957,7 @@
         </is>
       </c>
     </row>
-    <row r="234">
+    <row r="234" ht="69.75" customHeight="1">
       <c r="B234" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-24 213402.png</t>
@@ -11969,7 +11969,7 @@
         </is>
       </c>
     </row>
-    <row r="235">
+    <row r="235" ht="160.5" customHeight="1">
       <c r="B235" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-24 213440.png</t>
@@ -11981,7 +11981,7 @@
         </is>
       </c>
     </row>
-    <row r="236">
+    <row r="236" ht="46.5" customHeight="1">
       <c r="B236" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-24 220745.png</t>
@@ -11993,7 +11993,7 @@
         </is>
       </c>
     </row>
-    <row r="237">
+    <row r="237" ht="46.5" customHeight="1">
       <c r="B237" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-24 220811.png</t>
@@ -12005,7 +12005,7 @@
         </is>
       </c>
     </row>
-    <row r="238">
+    <row r="238" ht="46.5" customHeight="1">
       <c r="B238" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-24 220823.png</t>
@@ -12017,7 +12017,7 @@
         </is>
       </c>
     </row>
-    <row r="239">
+    <row r="239" ht="46.5" customHeight="1">
       <c r="B239" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-24 220844.png</t>
@@ -12029,7 +12029,7 @@
         </is>
       </c>
     </row>
-    <row r="240">
+    <row r="240" ht="42" customHeight="1">
       <c r="B240" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-26 103129.png</t>
@@ -12041,7 +12041,7 @@
         </is>
       </c>
     </row>
-    <row r="241">
+    <row r="241" ht="42" customHeight="1">
       <c r="B241" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-26 111009.png</t>
@@ -12053,7 +12053,7 @@
         </is>
       </c>
     </row>
-    <row r="242">
+    <row r="242" ht="42" customHeight="1">
       <c r="B242" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-26 144855.png</t>
@@ -12065,7 +12065,7 @@
         </is>
       </c>
     </row>
-    <row r="243">
+    <row r="243" ht="44.25" customHeight="1">
       <c r="B243" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-26 233927.png</t>
@@ -12077,7 +12077,7 @@
         </is>
       </c>
     </row>
-    <row r="244">
+    <row r="244" ht="30.75" customHeight="1">
       <c r="B244" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-30 153155.png</t>
@@ -12089,7 +12089,7 @@
         </is>
       </c>
     </row>
-    <row r="245">
+    <row r="245" ht="29.25" customHeight="1">
       <c r="B245" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-30 204130.png</t>
@@ -12101,7 +12101,7 @@
         </is>
       </c>
     </row>
-    <row r="246">
+    <row r="246" ht="45" customHeight="1">
       <c r="B246" t="inlineStr">
         <is>
           <t>Screenshot 2025-04-30 211540.png</t>
@@ -12113,7 +12113,7 @@
         </is>
       </c>
     </row>
-    <row r="247">
+    <row r="247" ht="46.5" customHeight="1">
       <c r="B247" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-02 161100.png</t>
@@ -12125,7 +12125,7 @@
         </is>
       </c>
     </row>
-    <row r="248">
+    <row r="248" ht="46.5" customHeight="1">
       <c r="B248" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-02 161735.png</t>
@@ -12137,7 +12137,7 @@
         </is>
       </c>
     </row>
-    <row r="249">
+    <row r="249" ht="18.75" customHeight="1">
       <c r="B249" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-06 003339.png</t>
@@ -12149,7 +12149,7 @@
         </is>
       </c>
     </row>
-    <row r="250">
+    <row r="250" ht="54.75" customHeight="1">
       <c r="B250" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-06 013856.png</t>
@@ -12161,7 +12161,7 @@
         </is>
       </c>
     </row>
-    <row r="251">
+    <row r="251" ht="62.25" customHeight="1">
       <c r="B251" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-06 014110.png</t>
@@ -12173,7 +12173,7 @@
         </is>
       </c>
     </row>
-    <row r="252">
+    <row r="252" ht="61.5" customHeight="1">
       <c r="B252" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-06 014244.png</t>
@@ -12185,7 +12185,7 @@
         </is>
       </c>
     </row>
-    <row r="253">
+    <row r="253" ht="67.5" customHeight="1">
       <c r="B253" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-06 041659.png</t>
@@ -12197,7 +12197,7 @@
         </is>
       </c>
     </row>
-    <row r="254">
+    <row r="254" ht="59.25" customHeight="1">
       <c r="B254" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-06 041811.png</t>
@@ -12209,7 +12209,7 @@
         </is>
       </c>
     </row>
-    <row r="255">
+    <row r="255" ht="72.75" customHeight="1">
       <c r="B255" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-06 041845.png</t>
@@ -12221,7 +12221,7 @@
         </is>
       </c>
     </row>
-    <row r="256">
+    <row r="256" ht="71.25" customHeight="1">
       <c r="B256" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-06 043302.png</t>
@@ -12233,7 +12233,7 @@
         </is>
       </c>
     </row>
-    <row r="257">
+    <row r="257" ht="45.75" customHeight="1">
       <c r="B257" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-06 111251.png</t>
@@ -12245,7 +12245,7 @@
         </is>
       </c>
     </row>
-    <row r="258">
+    <row r="258" ht="42" customHeight="1">
       <c r="B258" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-06 112725.png</t>
@@ -12257,7 +12257,7 @@
         </is>
       </c>
     </row>
-    <row r="259">
+    <row r="259" ht="91.5" customHeight="1">
       <c r="B259" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-08 152958.png</t>
@@ -12269,7 +12269,7 @@
         </is>
       </c>
     </row>
-    <row r="260">
+    <row r="260" ht="91.5" customHeight="1">
       <c r="B260" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-08 153921.png</t>
@@ -12281,7 +12281,7 @@
         </is>
       </c>
     </row>
-    <row r="261">
+    <row r="261" ht="93" customHeight="1">
       <c r="B261" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-08 154757.png</t>
@@ -12293,7 +12293,7 @@
         </is>
       </c>
     </row>
-    <row r="262">
+    <row r="262" ht="91.5" customHeight="1">
       <c r="B262" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-08 155812.png</t>
@@ -12305,7 +12305,7 @@
         </is>
       </c>
     </row>
-    <row r="263">
+    <row r="263" ht="91.5" customHeight="1">
       <c r="B263" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-08 161834.png</t>
@@ -12317,7 +12317,7 @@
         </is>
       </c>
     </row>
-    <row r="264">
+    <row r="264" ht="91.5" customHeight="1">
       <c r="B264" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-08 162047.png</t>
@@ -12329,7 +12329,7 @@
         </is>
       </c>
     </row>
-    <row r="265">
+    <row r="265" ht="92.25" customHeight="1">
       <c r="B265" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-08 163445.png</t>
@@ -12341,7 +12341,7 @@
         </is>
       </c>
     </row>
-    <row r="266">
+    <row r="266" ht="91.5" customHeight="1">
       <c r="B266" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-08 163457.png</t>
@@ -12353,7 +12353,7 @@
         </is>
       </c>
     </row>
-    <row r="267">
+    <row r="267" ht="91.5" customHeight="1">
       <c r="B267" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-08 163753.png</t>
@@ -12365,7 +12365,7 @@
         </is>
       </c>
     </row>
-    <row r="268">
+    <row r="268" ht="92.25" customHeight="1">
       <c r="B268" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-08 164212.png</t>
@@ -12377,7 +12377,7 @@
         </is>
       </c>
     </row>
-    <row r="269">
+    <row r="269" ht="92.25" customHeight="1">
       <c r="B269" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-08 164608.png</t>
@@ -12389,7 +12389,7 @@
         </is>
       </c>
     </row>
-    <row r="270">
+    <row r="270" ht="38.25" customHeight="1">
       <c r="B270" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-09 091947.png</t>
@@ -12401,7 +12401,7 @@
         </is>
       </c>
     </row>
-    <row r="271">
+    <row r="271" ht="23.25" customHeight="1">
       <c r="B271" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-09 155910.png</t>
@@ -12413,7 +12413,7 @@
         </is>
       </c>
     </row>
-    <row r="272">
+    <row r="272" ht="80.25" customHeight="1">
       <c r="B272" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-15 152505.png</t>
@@ -12425,7 +12425,7 @@
         </is>
       </c>
     </row>
-    <row r="273">
+    <row r="273" ht="79.5" customHeight="1">
       <c r="B273" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-15 152921.png</t>
@@ -12437,7 +12437,7 @@
         </is>
       </c>
     </row>
-    <row r="274">
+    <row r="274" ht="79.5" customHeight="1">
       <c r="B274" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-15 153101.png</t>
@@ -12449,7 +12449,7 @@
         </is>
       </c>
     </row>
-    <row r="275">
+    <row r="275" ht="79.5" customHeight="1">
       <c r="B275" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-15 153348.png</t>
@@ -12461,7 +12461,7 @@
         </is>
       </c>
     </row>
-    <row r="276">
+    <row r="276" ht="80.25" customHeight="1">
       <c r="B276" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-15 153435.png</t>
@@ -12473,7 +12473,7 @@
         </is>
       </c>
     </row>
-    <row r="277">
+    <row r="277" ht="80.25" customHeight="1">
       <c r="B277" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-15 153547.png</t>
@@ -12485,7 +12485,7 @@
         </is>
       </c>
     </row>
-    <row r="278">
+    <row r="278" ht="81" customHeight="1">
       <c r="B278" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-15 153736.png</t>
@@ -12497,7 +12497,7 @@
         </is>
       </c>
     </row>
-    <row r="279">
+    <row r="279" ht="80.25" customHeight="1">
       <c r="B279" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-15 153839.png</t>
@@ -12509,7 +12509,7 @@
         </is>
       </c>
     </row>
-    <row r="280">
+    <row r="280" ht="80.25" customHeight="1">
       <c r="B280" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-15 161358.png</t>
@@ -12521,7 +12521,7 @@
         </is>
       </c>
     </row>
-    <row r="281">
+    <row r="281" ht="79.5" customHeight="1">
       <c r="B281" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-15 161547.png</t>
@@ -12533,7 +12533,7 @@
         </is>
       </c>
     </row>
-    <row r="282">
+    <row r="282" ht="74.25" customHeight="1">
       <c r="B282" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-19 184906.png</t>
@@ -12545,7 +12545,7 @@
         </is>
       </c>
     </row>
-    <row r="283">
+    <row r="283" ht="69.75" customHeight="1">
       <c r="B283" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-20 125559.png</t>
@@ -12557,7 +12557,7 @@
         </is>
       </c>
     </row>
-    <row r="284">
+    <row r="284" ht="75" customHeight="1">
       <c r="B284" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-20 125828.png</t>
@@ -12569,7 +12569,7 @@
         </is>
       </c>
     </row>
-    <row r="285">
+    <row r="285" ht="42.75" customHeight="1">
       <c r="B285" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-20 130129.png</t>
@@ -12581,7 +12581,7 @@
         </is>
       </c>
     </row>
-    <row r="286">
+    <row r="286" ht="41.25" customHeight="1">
       <c r="B286" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-20 154258.png</t>
@@ -12593,7 +12593,7 @@
         </is>
       </c>
     </row>
-    <row r="287">
+    <row r="287" ht="45" customHeight="1">
       <c r="B287" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 151501.png</t>
@@ -12605,7 +12605,7 @@
         </is>
       </c>
     </row>
-    <row r="288">
+    <row r="288" ht="42" customHeight="1">
       <c r="B288" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 154112.png</t>
@@ -12617,7 +12617,7 @@
         </is>
       </c>
     </row>
-    <row r="289">
+    <row r="289" ht="42" customHeight="1">
       <c r="B289" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 154522.png</t>
@@ -12629,7 +12629,7 @@
         </is>
       </c>
     </row>
-    <row r="290">
+    <row r="290" ht="42" customHeight="1">
       <c r="B290" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 154544.png</t>
@@ -12641,7 +12641,7 @@
         </is>
       </c>
     </row>
-    <row r="291">
+    <row r="291" ht="41.25" customHeight="1">
       <c r="B291" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 154948.png</t>
@@ -12653,7 +12653,7 @@
         </is>
       </c>
     </row>
-    <row r="292">
+    <row r="292" ht="42.75" customHeight="1">
       <c r="B292" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 155016.png</t>
@@ -12665,7 +12665,7 @@
         </is>
       </c>
     </row>
-    <row r="293">
+    <row r="293" ht="32.25" customHeight="1">
       <c r="B293" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 160008.png</t>
@@ -12677,7 +12677,7 @@
         </is>
       </c>
     </row>
-    <row r="294">
+    <row r="294" ht="34.5" customHeight="1">
       <c r="B294" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 160132.png</t>
@@ -12689,7 +12689,7 @@
         </is>
       </c>
     </row>
-    <row r="295">
+    <row r="295" ht="39" customHeight="1">
       <c r="B295" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 160317.png</t>
@@ -12701,7 +12701,7 @@
         </is>
       </c>
     </row>
-    <row r="296">
+    <row r="296" ht="36" customHeight="1">
       <c r="B296" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 160938.png</t>
@@ -12713,7 +12713,7 @@
         </is>
       </c>
     </row>
-    <row r="297">
+    <row r="297" ht="42" customHeight="1">
       <c r="B297" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 161535.png</t>
@@ -12725,7 +12725,7 @@
         </is>
       </c>
     </row>
-    <row r="298">
+    <row r="298" ht="39" customHeight="1">
       <c r="B298" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 162030.png</t>
@@ -12737,7 +12737,7 @@
         </is>
       </c>
     </row>
-    <row r="299">
+    <row r="299" ht="39" customHeight="1">
       <c r="B299" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 162130.png</t>
@@ -12749,7 +12749,7 @@
         </is>
       </c>
     </row>
-    <row r="300">
+    <row r="300" ht="32.25" customHeight="1">
       <c r="B300" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 162738.png</t>
@@ -12761,7 +12761,7 @@
         </is>
       </c>
     </row>
-    <row r="301">
+    <row r="301" ht="42" customHeight="1">
       <c r="B301" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 163206.png</t>
@@ -12773,7 +12773,7 @@
         </is>
       </c>
     </row>
-    <row r="302">
+    <row r="302" ht="42" customHeight="1">
       <c r="B302" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 163855.png</t>
@@ -12785,7 +12785,7 @@
         </is>
       </c>
     </row>
-    <row r="303">
+    <row r="303" ht="32.25" customHeight="1">
       <c r="B303" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 164135.png</t>
@@ -12797,7 +12797,7 @@
         </is>
       </c>
     </row>
-    <row r="304">
+    <row r="304" ht="39.75" customHeight="1">
       <c r="B304" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 164209.png</t>
@@ -12809,7 +12809,7 @@
         </is>
       </c>
     </row>
-    <row r="305">
+    <row r="305" ht="36.75" customHeight="1">
       <c r="B305" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 164421.png</t>
@@ -12821,7 +12821,7 @@
         </is>
       </c>
     </row>
-    <row r="306">
+    <row r="306" ht="36.75" customHeight="1">
       <c r="B306" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 165226.png</t>
@@ -12833,7 +12833,7 @@
         </is>
       </c>
     </row>
-    <row r="307">
+    <row r="307" ht="40.5" customHeight="1">
       <c r="B307" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-22 165940.png</t>
@@ -12845,7 +12845,7 @@
         </is>
       </c>
     </row>
-    <row r="308">
+    <row r="308" ht="50.25" customHeight="1">
       <c r="B308" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-25 200403.png</t>
@@ -12857,7 +12857,7 @@
         </is>
       </c>
     </row>
-    <row r="309">
+    <row r="309" ht="87.75" customHeight="1">
       <c r="B309" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-27 123652.png</t>
@@ -12869,7 +12869,7 @@
         </is>
       </c>
     </row>
-    <row r="310">
+    <row r="310" ht="88.5" customHeight="1">
       <c r="B310" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-27 123727.png</t>
@@ -12881,7 +12881,7 @@
         </is>
       </c>
     </row>
-    <row r="311">
+    <row r="311" ht="87" customHeight="1">
       <c r="B311" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-27 123759.png</t>
@@ -12893,7 +12893,7 @@
         </is>
       </c>
     </row>
-    <row r="312">
+    <row r="312" ht="54.75" customHeight="1">
       <c r="B312" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-29 153716.png</t>
@@ -12905,7 +12905,7 @@
         </is>
       </c>
     </row>
-    <row r="313">
+    <row r="313" ht="54" customHeight="1">
       <c r="B313" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-29 154034.png</t>
@@ -12917,7 +12917,7 @@
         </is>
       </c>
     </row>
-    <row r="314">
+    <row r="314" ht="54" customHeight="1">
       <c r="B314" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-29 155712.png</t>
@@ -12929,7 +12929,7 @@
         </is>
       </c>
     </row>
-    <row r="315">
+    <row r="315" ht="51.75" customHeight="1">
       <c r="B315" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-29 160425.png</t>
@@ -12941,7 +12941,7 @@
         </is>
       </c>
     </row>
-    <row r="316">
+    <row r="316" ht="49.5" customHeight="1">
       <c r="B316" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-29 161104.png</t>
@@ -12953,7 +12953,7 @@
         </is>
       </c>
     </row>
-    <row r="317">
+    <row r="317" ht="47.25" customHeight="1">
       <c r="B317" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-29 161231.png</t>
@@ -12965,7 +12965,7 @@
         </is>
       </c>
     </row>
-    <row r="318">
+    <row r="318" ht="48" customHeight="1">
       <c r="B318" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-29 161937.png</t>
@@ -12977,7 +12977,7 @@
         </is>
       </c>
     </row>
-    <row r="319">
+    <row r="319" ht="51.75" customHeight="1">
       <c r="B319" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-29 162241.png</t>
@@ -12989,7 +12989,7 @@
         </is>
       </c>
     </row>
-    <row r="320">
+    <row r="320" ht="45" customHeight="1">
       <c r="B320" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-29 163345.png</t>
@@ -13001,7 +13001,7 @@
         </is>
       </c>
     </row>
-    <row r="321">
+    <row r="321" ht="59.25" customHeight="1">
       <c r="B321" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-29 164650.png</t>
@@ -13013,7 +13013,7 @@
         </is>
       </c>
     </row>
-    <row r="322">
+    <row r="322" ht="51" customHeight="1">
       <c r="B322" t="inlineStr">
         <is>
           <t>Screenshot 2025-05-29 165000.png</t>
@@ -13025,7 +13025,7 @@
         </is>
       </c>
     </row>
-    <row r="323">
+    <row r="323" ht="42.75" customHeight="1">
       <c r="B323" t="inlineStr">
         <is>
           <t>Screenshot 2025-06-03 204047.png</t>
@@ -13037,7 +13037,7 @@
         </is>
       </c>
     </row>
-    <row r="324">
+    <row r="324" ht="46.5" customHeight="1">
       <c r="B324" t="inlineStr">
         <is>
           <t>Screenshot 2025-06-07 190249.png</t>
@@ -13049,7 +13049,7 @@
         </is>
       </c>
     </row>
-    <row r="325">
+    <row r="325" ht="62.25" customHeight="1">
       <c r="B325" t="inlineStr">
         <is>
           <t>Screenshot 2025-06-09 220304.png</t>
@@ -13061,7 +13061,7 @@
         </is>
       </c>
     </row>
-    <row r="326">
+    <row r="326" ht="39" customHeight="1">
       <c r="B326" t="inlineStr">
         <is>
           <t>Screenshot 2025-06-11 231306.png</t>
@@ -13073,7 +13073,7 @@
         </is>
       </c>
     </row>
-    <row r="327">
+    <row r="327" ht="39.75" customHeight="1">
       <c r="B327" t="inlineStr">
         <is>
           <t>Screenshot 2025-06-12 141130.png</t>
@@ -13085,7 +13085,7 @@
         </is>
       </c>
     </row>
-    <row r="328">
+    <row r="328" ht="81" customHeight="1">
       <c r="B328" t="inlineStr">
         <is>
           <t>Screenshot 2025-06-13 194145.png</t>
@@ -13097,7 +13097,7 @@
         </is>
       </c>
     </row>
-    <row r="329">
+    <row r="329" ht="56.25" customHeight="1">
       <c r="B329" t="inlineStr">
         <is>
           <t>Screenshot 2025-06-27 132819.png</t>
@@ -13109,7 +13109,7 @@
         </is>
       </c>
     </row>
-    <row r="330">
+    <row r="330" ht="46.5" customHeight="1">
       <c r="B330" t="inlineStr">
         <is>
           <t>Screenshot 2025-07-10 202539.png</t>
@@ -13121,7 +13121,7 @@
         </is>
       </c>
     </row>
-    <row r="331">
+    <row r="331" ht="42.75" customHeight="1">
       <c r="B331" t="inlineStr">
         <is>
           <t>Screenshot 2025-07-16 233549.png</t>
@@ -13133,7 +13133,7 @@
         </is>
       </c>
     </row>
-    <row r="332">
+    <row r="332" ht="46.5" customHeight="1">
       <c r="B332" t="inlineStr">
         <is>
           <t>Screenshot 2025-07-18 185656.png</t>
@@ -13145,7 +13145,7 @@
         </is>
       </c>
     </row>
-    <row r="333">
+    <row r="333" ht="46.5" customHeight="1">
       <c r="B333" t="inlineStr">
         <is>
           <t>Screenshot 2025-07-20 174047.png</t>
@@ -13157,7 +13157,7 @@
         </is>
       </c>
     </row>
-    <row r="334">
+    <row r="334" ht="56.25" customHeight="1">
       <c r="B334" t="inlineStr">
         <is>
           <t>Screenshot 2025-07-23 131602.png</t>
@@ -13169,7 +13169,7 @@
         </is>
       </c>
     </row>
-    <row r="335">
+    <row r="335" ht="50.25" customHeight="1">
       <c r="B335" t="inlineStr">
         <is>
           <t>Screenshot 2025-07-23 132025.png</t>
@@ -13181,7 +13181,7 @@
         </is>
       </c>
     </row>
-    <row r="336">
+    <row r="336" ht="56.25" customHeight="1">
       <c r="B336" t="inlineStr">
         <is>
           <t>Screenshot 2025-07-23 132355.png</t>
@@ -13193,7 +13193,7 @@
         </is>
       </c>
     </row>
-    <row r="337">
+    <row r="337" ht="46.5" customHeight="1">
       <c r="B337" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-01 225639.png</t>
@@ -13205,7 +13205,7 @@
         </is>
       </c>
     </row>
-    <row r="338">
+    <row r="338" ht="78" customHeight="1">
       <c r="B338" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-02 200703.png</t>
@@ -13217,7 +13217,7 @@
         </is>
       </c>
     </row>
-    <row r="339">
+    <row r="339" ht="68.25" customHeight="1">
       <c r="B339" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-03 133018.png</t>
@@ -13229,7 +13229,7 @@
         </is>
       </c>
     </row>
-    <row r="340">
+    <row r="340" ht="92.25" customHeight="1">
       <c r="B340" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-03 154812.png</t>
@@ -13241,7 +13241,7 @@
         </is>
       </c>
     </row>
-    <row r="341">
+    <row r="341" ht="60" customHeight="1">
       <c r="B341" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-05 160007.png</t>
@@ -13253,7 +13253,7 @@
         </is>
       </c>
     </row>
-    <row r="342">
+    <row r="342" ht="49.5" customHeight="1">
       <c r="B342" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-05 160313.png</t>
@@ -13265,7 +13265,7 @@
         </is>
       </c>
     </row>
-    <row r="343">
+    <row r="343" ht="46.5" customHeight="1">
       <c r="B343" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-12 121830.png</t>
@@ -13277,7 +13277,7 @@
         </is>
       </c>
     </row>
-    <row r="344">
+    <row r="344" ht="46.5" customHeight="1">
       <c r="B344" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-12 221638.png</t>
@@ -13289,7 +13289,7 @@
         </is>
       </c>
     </row>
-    <row r="345">
+    <row r="345" ht="46.5" customHeight="1">
       <c r="B345" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-14 132720.png</t>
@@ -13301,7 +13301,7 @@
         </is>
       </c>
     </row>
-    <row r="346">
+    <row r="346" ht="46.5" customHeight="1">
       <c r="B346" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-16 173140.png</t>
@@ -13313,7 +13313,7 @@
         </is>
       </c>
     </row>
-    <row r="347">
+    <row r="347" ht="46.5" customHeight="1">
       <c r="B347" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-18 204837.png</t>
@@ -13325,7 +13325,7 @@
         </is>
       </c>
     </row>
-    <row r="348">
+    <row r="348" ht="107.25" customHeight="1">
       <c r="B348" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-18 214632.png</t>
@@ -13337,7 +13337,7 @@
         </is>
       </c>
     </row>
-    <row r="349">
+    <row r="349" ht="48.75" customHeight="1">
       <c r="B349" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-21 113833.png</t>
@@ -13349,7 +13349,7 @@
         </is>
       </c>
     </row>
-    <row r="350">
+    <row r="350" ht="60" customHeight="1">
       <c r="B350" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-26 102531.png</t>
@@ -13361,7 +13361,7 @@
         </is>
       </c>
     </row>
-    <row r="351">
+    <row r="351" ht="90.75" customHeight="1">
       <c r="B351" t="inlineStr">
         <is>
           <t>Screenshot 2025-08-26 154613.png</t>

</xml_diff>